<commit_message>
updated readme and temporarily finished analyzer
</commit_message>
<xml_diff>
--- a/out/AC 1421.xlsx
+++ b/out/AC 1421.xlsx
@@ -1220,7 +1220,7 @@
     <t>9% filler,90% QuantityHeader,</t>
   </si>
   <si>
-    <t>4% filler,47% SingleMassHeader,47% TotalMassHeader,</t>
+    <t>9% filler,90% TotalMassHeader,</t>
   </si>
   <si>
     <t>9% filler,90% containsProduct,</t>
@@ -1292,7 +1292,7 @@
     <t xml:space="preserve">VARENR  3, </t>
   </si>
   <si>
-    <t xml:space="preserve">VARENR  3, ANTAL 2, STK. MASSE 2, TOTAL MASSE 2</t>
+    <t xml:space="preserve">VARENR  3, ANTAL 2, STK. MASSE 1, TOTAL MASSE 2</t>
   </si>
   <si>
     <t xml:space="preserve">PRODUKT 1, </t>
@@ -1301,7 +1301,7 @@
     <t xml:space="preserve">ANTAL 2, </t>
   </si>
   <si>
-    <t>STK. MASSE 2, TOTAL MASSE 2</t>
+    <t>TOTAL MASSE 2</t>
   </si>
   <si>
     <t>varenavn oplyst</t>
@@ -2697,7 +2697,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFEB8C2"/>
+        <fgColor rgb="FFFEBAC2"/>
       </patternFill>
     </fill>
     <fill>
@@ -13496,7 +13496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DAF5EB4-63DF-4C50-9E7D-8969F8DEA662}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E882FEDE-277D-4808-BD8B-04F0AD7768C8}">
   <dimension ref="A1:I1179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
@@ -23723,7 +23723,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766ADEC5-D492-45DC-9CAB-6F524BB1CA7F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EFFA71-8A71-42E2-A1EA-5AF531140D6F}">
   <dimension ref="A1:H1179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
@@ -39449,7 +39449,7 @@
 </worksheet>
 </file>
 
-<file path=EPPlusLicense.txt>This workbook was created with the EPPlus library, licensed to Nikolaj R Christensen under the Polyform Noncommercial license, see https://polyformproject.org/licenses/noncommercial/1.0.0
-For more information about EPPlus, see https://epplussoftware.com/
+<file path=EPPlusLicense.txt>This workbook was created with the EPPlus library, licensed to Nikolaj R Christensen under the Polyform Noncommercial license, see https://polyformproject.org/licenses/noncommercial/1.0.0
+For more information about EPPlus, see https://epplussoftware.com/
 
 </file>
</xml_diff>